<commit_message>
Retirer la décote si l'impôt est déjà nul
</commit_message>
<xml_diff>
--- a/2022-08-11 - Calculateur Impôts - v3.xlsx
+++ b/2022-08-11 - Calculateur Impôts - v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Travail\Impots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B0C3E8C-6AD3-427D-92BA-823BBC9B7120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5D3DB3-B089-4992-BA19-E9119FE72C2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{87C24C3C-A098-47F3-B4F9-5793D4E9724F}"/>
+    <workbookView xWindow="5715" yWindow="-14715" windowWidth="19020" windowHeight="12690" xr2:uid="{87C24C3C-A098-47F3-B4F9-5793D4E9724F}"/>
   </bookViews>
   <sheets>
     <sheet name="Impôts 2021" sheetId="4" r:id="rId1"/>
@@ -1280,7 +1280,7 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1320,7 +1320,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="35">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -1328,19 +1328,19 @@
       <c r="D2" s="8"/>
       <c r="E2" s="10">
         <f>$A$4 + $A$6</f>
-        <v>60000</v>
+        <v>0</v>
       </c>
       <c r="F2" s="10">
         <f>$A$4 + $A$6</f>
-        <v>60000</v>
+        <v>0</v>
       </c>
       <c r="G2" s="10">
         <f>$A$4 + $A$6</f>
-        <v>60000</v>
+        <v>0</v>
       </c>
       <c r="H2" s="10">
         <f>$A$4 + $A$6</f>
-        <v>60000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -1355,19 +1355,19 @@
       </c>
       <c r="E3" s="10">
         <f>E2 * $D$3</f>
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="F3" s="10">
         <f>F2 * $D$3</f>
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="G3" s="10">
         <f>G2 * $D$3</f>
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="H3" s="10">
         <f>H2 * $D$3</f>
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="K3" s="20"/>
       <c r="L3" s="1" t="s">
@@ -1376,7 +1376,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="34">
-        <v>25000</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
@@ -1384,19 +1384,19 @@
       <c r="D4" s="8"/>
       <c r="E4" s="10">
         <f>E2 - E3</f>
-        <v>54000</v>
+        <v>0</v>
       </c>
       <c r="F4" s="10">
         <f>F2 - F3</f>
-        <v>54000</v>
+        <v>0</v>
       </c>
       <c r="G4" s="10">
         <f>G2 - G3</f>
-        <v>54000</v>
+        <v>0</v>
       </c>
       <c r="H4" s="10">
         <f>H2 - H3</f>
-        <v>54000</v>
+        <v>0</v>
       </c>
       <c r="K4" s="27"/>
       <c r="L4" s="1" t="s">
@@ -1415,19 +1415,19 @@
       </c>
       <c r="E5" s="10">
         <f>E4 - $D$5</f>
-        <v>54000</v>
+        <v>0</v>
       </c>
       <c r="F5" s="10">
         <f>F4 - $D$5</f>
-        <v>54000</v>
+        <v>0</v>
       </c>
       <c r="G5" s="10">
         <f>G4 - $D$5</f>
-        <v>54000</v>
+        <v>0</v>
       </c>
       <c r="H5" s="10">
         <f>H4 - $D$5</f>
-        <v>54000</v>
+        <v>0</v>
       </c>
       <c r="K5" s="30"/>
       <c r="L5" s="1" t="s">
@@ -1436,7 +1436,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="34">
-        <v>35000</v>
+        <v>0</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>30</v>
@@ -1472,47 +1472,47 @@
       <c r="D7" s="32"/>
       <c r="E7" s="10">
         <f>E5-E6</f>
-        <v>54000</v>
+        <v>0</v>
       </c>
       <c r="F7" s="10">
         <f>F5-F6</f>
-        <v>54000</v>
+        <v>0</v>
       </c>
       <c r="G7" s="10">
         <f>G5-G6</f>
-        <v>54000</v>
+        <v>0</v>
       </c>
       <c r="H7" s="10">
         <f>H5-H6</f>
-        <v>54000</v>
+        <v>0</v>
       </c>
       <c r="K7" s="33"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E8" s="17">
         <f>E7 / $D$8</f>
-        <v>27000</v>
+        <v>0</v>
       </c>
       <c r="F8" s="17">
         <f>F7 / $D$8</f>
-        <v>27000</v>
+        <v>0</v>
       </c>
       <c r="G8" s="17">
         <f>G7 / $D$8</f>
-        <v>27000</v>
+        <v>0</v>
       </c>
       <c r="H8" s="17">
         <f>H7 / $D$8</f>
-        <v>27000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -1525,11 +1525,11 @@
       <c r="E9" s="5"/>
       <c r="F9" s="10">
         <f>(A2/$D$20) /$D$8</f>
-        <v>6250</v>
+        <v>0</v>
       </c>
       <c r="G9" s="10">
         <f xml:space="preserve"> (A2-(A2*D9)) / $D$8</f>
-        <v>12500</v>
+        <v>0</v>
       </c>
       <c r="H9" s="4"/>
     </row>
@@ -1545,11 +1545,11 @@
       <c r="F10" s="4"/>
       <c r="G10" s="11">
         <f>A2</f>
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="H10" s="10">
         <f xml:space="preserve"> A2</f>
-        <v>50000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -1562,19 +1562,19 @@
       <c r="D11" s="13"/>
       <c r="E11" s="14">
         <f>E8+E9</f>
-        <v>27000</v>
+        <v>0</v>
       </c>
       <c r="F11" s="14">
         <f>F8+F9</f>
-        <v>33250</v>
+        <v>0</v>
       </c>
       <c r="G11" s="14">
         <f>G8+G9</f>
-        <v>39500</v>
+        <v>0</v>
       </c>
       <c r="H11" s="14">
         <f>H8+H9</f>
-        <v>27000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -1612,19 +1612,19 @@
       </c>
       <c r="E13" s="10">
         <f>IF(E11-$C$12&gt;0,IF(E11&gt;$C$13,($C$13-$C$12)*$D$13,(E11-$C$12)*$D$13),0)</f>
-        <v>1742.95</v>
+        <v>0</v>
       </c>
       <c r="F13" s="10">
         <f>IF(F11-$C$12&gt;0,IF(F11&gt;$C$13,($C$13-$C$12)*$D$13,(F11-$C$12)*$D$13),0)</f>
-        <v>1742.95</v>
+        <v>0</v>
       </c>
       <c r="G13" s="10">
         <f>IF(G11-$C$12&gt;0,IF(G11&gt;$C$13,($C$13-$C$12)*$D$13,(G11-$C$12)*$D$13),0)</f>
-        <v>1742.95</v>
+        <v>0</v>
       </c>
       <c r="H13" s="10">
         <f>IF(H11-$C$12&gt;0,IF(H11&gt;$C$13,($C$13-$C$12)*$D$13,(H11-$C$12)*$D$13),0)</f>
-        <v>1742.95</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -1639,19 +1639,19 @@
       </c>
       <c r="E14" s="10">
         <f>IF(E11-$C$13&gt;0,IF(E11&gt;$C$14,($C$14-$C$13)*$D$14,(E11-$C$13)*$D$14),0)</f>
-        <v>279</v>
+        <v>0</v>
       </c>
       <c r="F14" s="10">
         <f>IF(F11-$C$13&gt;0,IF(F11&gt;$C$14,($C$14-$C$13)*$D$14,(F11-$C$13)*$D$14),0)</f>
-        <v>2154</v>
+        <v>0</v>
       </c>
       <c r="G14" s="10">
         <f>IF(G11-$C$13&gt;0,IF(G11&gt;$C$14,($C$14-$C$13)*$D$14,(G11-$C$13)*$D$14),0)</f>
-        <v>4029</v>
+        <v>0</v>
       </c>
       <c r="H14" s="10">
         <f>IF(H11-$C$13&gt;0,IF(H11&gt;$C$14,($C$14-$C$13)*$D$14,(H11-$C$13)*$D$14),0)</f>
-        <v>279</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -1716,19 +1716,19 @@
       <c r="D17" s="13"/>
       <c r="E17" s="14">
         <f>SUM(E12:E16) *  $D$8</f>
-        <v>4043.9</v>
+        <v>0</v>
       </c>
       <c r="F17" s="14">
         <f>SUM(F12:F16) * $D$8</f>
-        <v>7793.9</v>
+        <v>0</v>
       </c>
       <c r="G17" s="14">
         <f>SUM(G12:G16) *  $D$8</f>
-        <v>11543.9</v>
+        <v>0</v>
       </c>
       <c r="H17" s="15">
         <f>SUM(H12:H16) *  $D$8</f>
-        <v>4043.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -1742,19 +1742,19 @@
         <v>0.45250000000000001</v>
       </c>
       <c r="E18" s="10">
-        <f>IF($A$8="Couple",IF(E17 &lt;$A$20,($A$18 - ($D$18 * E17)),0),IF(E17 &lt;$A$15,($A$13 - ($D$18 * E17)),0))</f>
+        <f>IF(E17&gt;0,IF($A$8="Couple",IF(E17 &lt;$A$20,($A$18 - ($D$18 * E17)),0),IF(E17 &lt;$A$15,($A$13 - ($D$18 * E17)),0)),0)</f>
         <v>0</v>
       </c>
       <c r="F18" s="10">
-        <f>IF($A$8="Couple",IF(F17 &lt;$A$20,($A$18 - ($D$18 * F17)),0),IF(F17 &lt;$A$15,($A$13 - ($D$18 * F17)),0))</f>
+        <f>IF(F17&gt;0,IF($A$8="Couple",IF(F17 &lt;$A$20,($A$18 - ($D$18 * F17)),0),IF(F17 &lt;$A$15,($A$13 - ($D$18 * F17)),0)),0)</f>
         <v>0</v>
       </c>
       <c r="G18" s="10">
-        <f>IF($A$8="Couple",IF(G17 &lt;$A$20,($A$18 - ($D$18 * G17)),0),IF(G17 &lt;$A$15,($A$13 - ($D$18 * G17)),0))</f>
+        <f>IF(G17&gt;0,IF($A$8="Couple",IF(G17 &lt;$A$20,($A$18 - ($D$18 * G17)),0),IF(G17 &lt;$A$15,($A$13 - ($D$18 * G17)),0)),0)</f>
         <v>0</v>
       </c>
       <c r="H18" s="10">
-        <f>IF($A$8="Couple",IF(H17 &lt;$A$20,($A$18 - ($D$18 * H17)),0),IF(H17 &lt;$A$15,($A$13 - ($D$18 * H17)),0))</f>
+        <f>IF(H17&gt;0,IF($A$8="Couple",IF(H17 &lt;$A$20,($A$18 - ($D$18 * H17)),0),IF(H17 &lt;$A$15,($A$13 - ($D$18 * H17)),0)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1767,23 +1767,23 @@
       </c>
       <c r="D19" s="28">
         <f>IF($A$8="Couple",$A$18,$A$13)</f>
-        <v>1307</v>
+        <v>790</v>
       </c>
       <c r="E19" s="10">
         <f>IF((E17-E18)&gt;0,E17-E18,0)</f>
-        <v>4043.9</v>
+        <v>0</v>
       </c>
       <c r="F19" s="10">
         <f>IF((F17-F18)&gt;0,F17-F18,0)</f>
-        <v>7793.9</v>
+        <v>0</v>
       </c>
       <c r="G19" s="10">
         <f>IF((G17-G18)&gt;0,G17-G18,0)</f>
-        <v>11543.9</v>
+        <v>0</v>
       </c>
       <c r="H19" s="10">
         <f>IF((H17-H18)&gt;0,H17-H18,0)</f>
-        <v>4043.9</v>
+        <v>0</v>
       </c>
       <c r="J19" s="7"/>
     </row>
@@ -1800,7 +1800,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="10">
         <f>E19 + ((F19-E19)*$D$20)</f>
-        <v>19043.899999999998</v>
+        <v>0</v>
       </c>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
@@ -1816,11 +1816,11 @@
       <c r="F21" s="4"/>
       <c r="G21" s="10">
         <f>G10 *$D$21</f>
-        <v>8600</v>
+        <v>0</v>
       </c>
       <c r="H21" s="10">
         <f>H10 *$D$21</f>
-        <v>8600</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -1835,7 +1835,7 @@
       <c r="G22" s="5"/>
       <c r="H22" s="10">
         <f>H10 *$D$22</f>
-        <v>6400</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -1850,11 +1850,11 @@
       <c r="F23" s="5"/>
       <c r="G23" s="10">
         <f>G21+G22</f>
-        <v>8600</v>
+        <v>0</v>
       </c>
       <c r="H23" s="10">
         <f>H21+H22</f>
-        <v>15000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -1864,19 +1864,19 @@
       <c r="D24" s="13"/>
       <c r="E24" s="14">
         <f>E19+E23</f>
-        <v>4043.9</v>
+        <v>0</v>
       </c>
       <c r="F24" s="14">
         <f>F20+F23</f>
-        <v>19043.899999999998</v>
+        <v>0</v>
       </c>
       <c r="G24" s="14">
         <f>G19+G23</f>
-        <v>20143.900000000001</v>
+        <v>0</v>
       </c>
       <c r="H24" s="15">
         <f>H19+H23</f>
-        <v>19043.900000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -1888,19 +1888,19 @@
       </c>
       <c r="E25" s="10">
         <f>E24-$D$25</f>
-        <v>4043.9</v>
+        <v>0</v>
       </c>
       <c r="F25" s="10">
         <f>F24-$D$25</f>
-        <v>19043.899999999998</v>
+        <v>0</v>
       </c>
       <c r="G25" s="10">
         <f>G24-$D$25</f>
-        <v>20143.900000000001</v>
+        <v>0</v>
       </c>
       <c r="H25" s="10">
         <f>H24-$D$25</f>
-        <v>19043.900000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -1912,19 +1912,19 @@
       </c>
       <c r="E26" s="10">
         <f>E25+ $D$26</f>
-        <v>4043.9</v>
+        <v>0</v>
       </c>
       <c r="F26" s="10">
         <f>F25+ $D$26</f>
-        <v>19043.899999999998</v>
+        <v>0</v>
       </c>
       <c r="G26" s="10">
         <f>G25+ $D$26</f>
-        <v>20143.900000000001</v>
+        <v>0</v>
       </c>
       <c r="H26" s="10">
         <f>H25+ $D$26</f>
-        <v>19043.900000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -1936,19 +1936,19 @@
       </c>
       <c r="E27" s="10">
         <f>E25-$D$27</f>
-        <v>4043.9</v>
+        <v>0</v>
       </c>
       <c r="F27" s="10">
         <f>F25-$D$27</f>
-        <v>19043.899999999998</v>
+        <v>0</v>
       </c>
       <c r="G27" s="10">
         <f>G25-$D$27</f>
-        <v>20143.900000000001</v>
+        <v>0</v>
       </c>
       <c r="H27" s="10">
         <f>H25-$D$27</f>
-        <v>19043.900000000001</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>